<commit_message>
[AV] Mechanoid Spots 번역 갱신 및 공백 오류 수정
</commit_message>
<xml_diff>
--- a/Data/[AV] Mechanoid Spots - 3238521451/[AV] Mechanoid Spots - 3238521451.xlsx
+++ b/Data/[AV] Mechanoid Spots - 3238521451/[AV] Mechanoid Spots - 3238521451.xlsx
@@ -5,22 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zilrt\Desktop\추가\[AV] Mechanoid Spots - 3238521451\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\[AV] Mechanoid Spots - 3238521451\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A045CA-4109-43D8-8449-F0B738468D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7605A8B3-7AC7-48FD-8BA9-320411D1E917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="518">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -52,9 +65,6 @@
     <t>mech socket</t>
   </si>
   <si>
-    <t>메카노이드 소켓</t>
-  </si>
-  <si>
     <t>ThingDef+AV_Mechworkstation.description</t>
   </si>
   <si>
@@ -74,9 +84,6 @@
   </si>
   <si>
     <t>work mode</t>
-  </si>
-  <si>
-    <t>작업 모드</t>
   </si>
   <si>
     <t>HediffDef+AV_MechWorkBoost.description</t>
@@ -325,18 +332,6 @@
     <t>HediffDef+AV_FluoidBoost.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>플루오이드용으로 특별히 설계된 메카노이드 작업 스테이션입니다. 위에 지정된 메카노이드와 연결되어 플루오이드 재처리를 지원하며, 전력 생성기의 부하를 줄여 독성 폐기물을 줄이고 신경포말 생산을 가속화합니다. 근처의 다른 메카노이드 작업 스테이션과 간섭하며 전선에 직접 연결이 필요합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>AV_FluoidBoost.label</t>
   </si>
   <si>
@@ -1045,19 +1040,10 @@
     <t>colored mechlink range needs to be activated in [AV] Core Framework settings</t>
   </si>
   <si>
-    <t>[AV] 코어 프레임워크 설정에서 활성화해야 하는 색상 메크링크 범위</t>
-  </si>
-  <si>
     <t>Keyed+AV_SettingsBoxReason_ColorFromFramework</t>
   </si>
   <si>
     <t>AV_SettingsBoxReason_ColorFromFramework</t>
-  </si>
-  <si>
-    <t>[AV] Core Framework settings</t>
-  </si>
-  <si>
-    <t>[AV] 코어 프레임워크 설정</t>
   </si>
   <si>
     <t>Keyed+AV_SettingsBoxLabel_PsychicDisturber</t>
@@ -1414,111 +1400,369 @@
     <t>폐기물 생산이 활성화되어야 하며, 그렇지 않으면 이 설정은 아무런 효과가 없습니다.</t>
   </si>
   <si>
-    <t xml:space="preserve">방수 메카노이드 작업 스테이션으로, 작업 메카노이드의 효율을 높이기 위해 설계되었습니다. 이 스테이션은 소켓 위의 모든 메카노이드와 연결되어 성능을 최적화하고 에너지 소비율을 줄임으로써 시간이 지남에 따라 독성 폐기물 배출을 줄입니다. 그러나 주변의 다른 메카노이드 작업 스테이션과 간섭이 발생할 수 있으며, 전력 공급 라인에 직접 연결되어야 합니다.
-</t>
+    <t>메카노이드 지점</t>
+  </si>
+  <si>
+    <t>신호 분배기가 있는 단순 디스크입니다. 이 신호는 지정된 메카노이드를 특정 지점으로 이동시키는 데 사용할 수 있습니다. 적은 전력이 필요합니다.</t>
+  </si>
+  <si>
+    <t>고정 메카노이드 지점</t>
+  </si>
+  <si>
+    <t>고정된 신호 분배기입니다. 이 신호는 지정된 메카노이드를 특정 지점으로 이동시키는 데 사용할 수 있습니다. 적은 전력이 필요합니다.</t>
+  </si>
+  <si>
+    <t>지정된 지점에 머물기</t>
+  </si>
+  <si>
+    <t>작고 전기적으로 충전된 돌로, 정성스럽게 연마되고 조각되어 사용 가능한 에너지 흐름을 만듭니다. 약한 펄스 신호는 메카노이드의 표시 지점으로 작동하기에 충분합니다.</t>
+  </si>
+  <si>
+    <t>이 지점을 특정 메카에 할당</t>
+  </si>
+  <si>
+    <t>체크됨: \n시야 내 쓰러진 적을 무시하고 지점을 유지합니다. \n체크 해제됨: \n지도에서 적이 감지되면(쓰러진 적 포함) 메카가 순찰을 시작할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>체크됨: \n지정된 메카는 다른 충전기가 없을 때 이 지점에서 휴면 충전을 할 수 있습니다(충전 설정에 따라 다름) \n체크 해제됨: \n지정된 메카는 이 지점을 충전 지점으로 간주하지 않습니다.</t>
+  </si>
+  <si>
+    <t>이 지점의 설정을 클립보드에 복사하여 다른 지점에 붙여넣을 수 있습니다.</t>
+  </si>
+  <si>
+    <t>이 지점의 설정을 이전에 클립보드에 복사한 설정으로 덮어씁니다.</t>
+  </si>
+  <si>
+    <t>지점에서 충전 중</t>
+  </si>
+  <si>
+    <t>지점에서 경비 중</t>
+  </si>
+  <si>
+    <t>지점에서 생산 중</t>
+  </si>
+  <si>
+    <t>지점에 머무는 중</t>
+  </si>
+  <si>
+    <t>근처 지점에 {0}(을)를 운반할 수 없습니다: {0}에는 지점이 없습니다.</t>
+  </si>
+  <si>
+    <t>근처 지점에 {0}(을)를 운반할 수 없습니다</t>
+  </si>
+  <si>
+    <t>{0}(을)를 자신의 지점으로 운반</t>
+  </si>
+  <si>
+    <t>지점에 대한 메카 기록</t>
+  </si>
+  <si>
+    <t>메카노이드 지점에 할당된 오버레이 표시</t>
+  </si>
+  <si>
+    <t>메카 지점에서 할당된 메카의 이름을 표시합니다.</t>
+  </si>
+  <si>
+    <t>메카노이드 지점에 할당되지 않은 오버레이 표시</t>
+  </si>
+  <si>
+    <t>할당되지 않은 메카 지점에 할당되지 않은 레이블을 표시합니다.</t>
+  </si>
+  <si>
+    <t>노랑 = 메카가 죽음\n빨강 = 메카가 파괴되어 로딩 후 지점에서 해제됩니다</t>
+  </si>
+  <si>
+    <t>타일에 지점을 맞춥니다(재시작 필요)</t>
+  </si>
+  <si>
+    <t>지점이 하단으로 치우치는 것이 마음에 들지 않으면 이 옵션을 체크하십시오.</t>
+  </si>
+  <si>
+    <t>기본 지점 설정: 지점에서 메카가 휴면 충전할 수 있도록 허용</t>
+  </si>
+  <si>
+    <t>새로 생성된 지점은 기본값으로 사용됩니다. 이미 생성된 지점은 변경되지 않습니다.</t>
+  </si>
+  <si>
+    <t>대는 메카노이드 지점을 사용할 수 있습니다</t>
+  </si>
+  <si>
+    <t>전력 없이도 지점을 사용할 수 있도록 허용</t>
+  </si>
+  <si>
+    <t>모든 지점</t>
+  </si>
+  <si>
+    <t>[AV] Mechtech</t>
+  </si>
+  <si>
+    <t>프레임워크 설정: 소켓과 대역폭 확장기를 위한 정신 교란기 플레이스워커 사용</t>
+  </si>
+  <si>
+    <t>방수 메카노이드 작업 스테이션으로, 작업 메카노이드의 효율을 높이기 위해 설계되었습니다. 이 스테이션은 소켓 위의 모든 메카노이드와 연결되어 성능을 최적화하고 에너지 소비율을 줄임으로써 시간이 지남에 따라 독성 폐기물 배출을 줄입니다. 그러나 주변의 다른 메카노이드 작업 스테이션과 간섭이 발생할 수 있으며, 전력 공급 라인에 직접 연결되어야 합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>메카노이드 지점</t>
-  </si>
-  <si>
-    <t>신호 분배기가 있는 단순 디스크입니다. 이 신호는 지정된 메카노이드를 특정 지점으로 이동시키는 데 사용할 수 있습니다. 적은 전력이 필요합니다.</t>
-  </si>
-  <si>
-    <t>고정 메카노이드 지점</t>
-  </si>
-  <si>
-    <t>고정된 신호 분배기입니다. 이 신호는 지정된 메카노이드를 특정 지점으로 이동시키는 데 사용할 수 있습니다. 적은 전력이 필요합니다.</t>
-  </si>
-  <si>
-    <t>지정된 지점에 머물기</t>
-  </si>
-  <si>
-    <t>작고 전기적으로 충전된 돌로, 정성스럽게 연마되고 조각되어 사용 가능한 에너지 흐름을 만듭니다. 약한 펄스 신호는 메카노이드의 표시 지점으로 작동하기에 충분합니다.</t>
-  </si>
-  <si>
-    <t>이 지점을 특정 메카에 할당</t>
-  </si>
-  <si>
-    <t>체크됨: \n시야 내 쓰러진 적을 무시하고 지점을 유지합니다. \n체크 해제됨: \n지도에서 적이 감지되면(쓰러진 적 포함) 메카가 순찰을 시작할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>체크됨: \n지정된 메카는 다른 충전기가 없을 때 이 지점에서 휴면 충전을 할 수 있습니다(충전 설정에 따라 다름) \n체크 해제됨: \n지정된 메카는 이 지점을 충전 지점으로 간주하지 않습니다.</t>
-  </si>
-  <si>
-    <t>이 지점의 설정을 클립보드에 복사하여 다른 지점에 붙여넣을 수 있습니다.</t>
-  </si>
-  <si>
-    <t>이 지점의 설정을 이전에 클립보드에 복사한 설정으로 덮어씁니다.</t>
-  </si>
-  <si>
-    <t>지점에서 충전 중</t>
-  </si>
-  <si>
-    <t>지점에서 경비 중</t>
-  </si>
-  <si>
-    <t>지점에서 생산 중</t>
-  </si>
-  <si>
-    <t>지점에 머무는 중</t>
-  </si>
-  <si>
-    <t>근처 지점에 {0}(을)를 운반할 수 없습니다: {0}에는 지점이 없습니다.</t>
-  </si>
-  <si>
-    <t>근처 지점에 {0}(을)를 운반할 수 없습니다</t>
-  </si>
-  <si>
-    <t>{0}(을)를 자신의 지점으로 운반</t>
-  </si>
-  <si>
-    <t>지점에 대한 메카 기록</t>
-  </si>
-  <si>
-    <t>메카노이드 지점에 할당된 오버레이 표시</t>
-  </si>
-  <si>
-    <t>메카 지점에서 할당된 메카의 이름을 표시합니다.</t>
-  </si>
-  <si>
-    <t>메카노이드 지점에 할당되지 않은 오버레이 표시</t>
-  </si>
-  <si>
-    <t>할당되지 않은 메카 지점에 할당되지 않은 레이블을 표시합니다.</t>
-  </si>
-  <si>
-    <t>노랑 = 메카가 죽음\n빨강 = 메카가 파괴되어 로딩 후 지점에서 해제됩니다</t>
-  </si>
-  <si>
-    <t>타일에 지점을 맞춥니다(재시작 필요)</t>
-  </si>
-  <si>
-    <t>지점이 하단으로 치우치는 것이 마음에 들지 않으면 이 옵션을 체크하십시오.</t>
-  </si>
-  <si>
-    <t>기본 지점 설정: 지점에서 메카가 휴면 충전할 수 있도록 허용</t>
-  </si>
-  <si>
-    <t>새로 생성된 지점은 기본값으로 사용됩니다. 이미 생성된 지점은 변경되지 않습니다.</t>
-  </si>
-  <si>
-    <t>대는 메카노이드 지점을 사용할 수 있습니다</t>
-  </si>
-  <si>
-    <t>전력 없이도 지점을 사용할 수 있도록 허용</t>
-  </si>
-  <si>
-    <t>모든 지점</t>
-  </si>
-  <si>
     <t>A rainproof mechanoid work station designed to improve the efficiency of mechanoid workers. It connects to any mechanoid on top, optimizing the performance and reducing the energy consumption rate, resulting in less toxic waste over time. It interferes with other mechanoid workstations in the vicinity and requires a direct connection to a power conduit.</t>
-  </si>
-  <si>
-    <t>[AV] Mechtech</t>
-  </si>
-  <si>
-    <t>프레임워크 설정: 소켓과 대역폭 확장기를 위한 정신 교란기 플레이스워커 사용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드 소켓</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업 모드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플루오이드용으로 특별히 설계된 메카노이드 작업 스테이션입니다. 위에 지정된 메카노이드와 연결되어 플루오이드 재처리를 지원하며, 전력 생성기의 부하를 줄여 독성 폐기물을 줄이고 뉴로폼 생산을 가속화합니다. 근처의 다른 메카노이드 작업 스테이션과 간섭하며 전선에 직접 연결이 필요합니다.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResearchProjectDef</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.label</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.description</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>AV_Machanoid_Sockets.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.label</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.description</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>AV_Pulse_Charger.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>AV_Research.label</t>
+  </si>
+  <si>
+    <t>AV_Research.generalDescription</t>
+  </si>
+  <si>
+    <t>AV_Research.generalTitle</t>
+  </si>
+  <si>
+    <t>ResearchTabDef</t>
+  </si>
+  <si>
+    <t>subject-&gt;mechanoid sockets</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;visited a mechanoid driven glitterworld</t>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;worked in a glitterworld research facility to improve living standards</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;experimented with mechanoid tech</t>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;socketing mechanoids</t>
+  </si>
+  <si>
+    <t>subject-&gt;pulse charger</t>
+  </si>
+  <si>
+    <t>subject-&gt;mechanoid cells</t>
+  </si>
+  <si>
+    <t>mechanoid sockets</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use basic subcores to build mechanoid stations.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pulse charger</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charge mechanoids with regular pulses of electrical energy. Although this special process is not as fast as conventional charging, it does not produce any toxic waste.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mechtech</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unlock technologies from [AV] Mods by researching at a research bench, mostly centered around mechtech.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[AV] Mechtech research projects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.label</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.description</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Machanoid_Sockets.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.label</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.description</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+AV_Pulse_Charger.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>ResearchTabDef+AV_Research.label</t>
+  </si>
+  <si>
+    <t>ResearchTabDef+AV_Research.generalDescription</t>
+  </si>
+  <si>
+    <t>ResearchTabDef+AV_Research.generalTitle</t>
+  </si>
+  <si>
+    <t>subject-&gt;메카노이드 소켓</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>펄스 충전기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject-&gt;펄스 충전기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject-&gt;메카노이드 셀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메크테크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[AV] Mechtech 연구 프로젝트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;메카노이드 소켓팅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;메카노이드 기술 실험</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;생활 수준 향상을 위해 번화계 연구 시설에서 근무</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;메카노이드가 운영하는 번화계 방문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전기 에너지의 규칙적인 펄스로 메카노이드를 충전합니다. 이 특수 공정은 기존 충전만큼 빠르지는 않지만 독성 폐기물을 생산하지 않습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드 스테이션을 만들기 위해 기본 서브코어 사용.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[AV] Core Framework settings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[AV] Core Framework 설정에서 활성화해야 하는 색상 메크링크 범위</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[AV] Core Framework 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patrolling.</t>
+  </si>
+  <si>
+    <t>ThinkTreeDef</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mechanoid.thinkRoot.subNodes.7.subNodes.0.subNodes.1.subNodes.4.subNodes.2.subNodes.0.reportStringOverride</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThinkTreeDef+Mechanoid.thinkRoot.subNodes.7.subNodes.0.subNodes.1.subNodes.4.subNodes.2.subNodes.0.reportStringOverride</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구 작업대에서 연구하여 [AV] 모드의 기술을 잠금 해제, 주로 메크테크를 중심으로 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>순찰 중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1882,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD100"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1934,1895 +2178,2218 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="132" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>413</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>89</v>
+        <v>444</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="F62" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="F65" s="1" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="F72" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="F84" s="1" t="s">
-        <v>311</v>
+        <v>510</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>314</v>
+        <v>509</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>315</v>
+        <v>511</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="F100" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F101" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F102" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="F103" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="F104" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="F105" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="F106" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="F107" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="F108" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="F109" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="F110" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="F111" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F112" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>